<commit_message>
fix vitamin in store text
</commit_message>
<xml_diff>
--- a/text/store.xlsx
+++ b/text/store.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="110">
   <si>
     <t xml:space="preserve">7E
 *
@@ -254,31 +254,39 @@
 8C</t>
   </si>
   <si>
+    <t xml:space="preserve">P
+1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z
+24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7A
+O
+19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J
+14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74
+V
+20</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ĉ
 1B</t>
   </si>
   <si>
-    <t xml:space="preserve">7A
-A
-0B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P
-1A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74
-E
-0F</t>
-  </si>
-  <si>
     <t xml:space="preserve">72
-Z
-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J
-14</t>
+T
+1E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72
+00</t>
   </si>
   <si>
     <t xml:space="preserve">K
@@ -289,8 +297,11 @@
 00</t>
   </si>
   <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
     <t xml:space="preserve">52
-EB</t>
+EC</t>
   </si>
   <si>
     <t xml:space="preserve">V
@@ -331,8 +342,9 @@
 2B</t>
   </si>
   <si>
-    <t xml:space="preserve">I
-F1</t>
+    <t xml:space="preserve">46
+I
+F2</t>
   </si>
   <si>
     <t xml:space="preserve">6A
@@ -345,29 +357,6 @@
 0D</t>
   </si>
   <si>
-    <t xml:space="preserve">Z
-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7A
-O
-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74
-V
-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72
-T
-1E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72
-00</t>
-  </si>
-  <si>
     <t xml:space="preserve">6A</t>
   </si>
   <si>
@@ -440,7 +429,7 @@
     <t xml:space="preserve">50</t>
   </si>
   <si>
-    <t xml:space="preserve">EB</t>
+    <t xml:space="preserve">EC</t>
   </si>
   <si>
     <t xml:space="preserve">64</t>
@@ -452,7 +441,7 @@
     <t xml:space="preserve">76</t>
   </si>
   <si>
-    <t xml:space="preserve">51</t>
+    <t xml:space="preserve">F2</t>
   </si>
   <si>
     <t xml:space="preserve">0D</t>
@@ -586,7 +575,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,6 +617,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -716,10 +713,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF38"/>
+  <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G18" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1407,40 +1404,40 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>1</v>
@@ -1505,43 +1502,43 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="L11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>1</v>
@@ -1606,7 +1603,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>26</v>
@@ -1618,7 +1615,7 @@
         <v>7</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>6</v>
@@ -1689,7 +1686,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1705,7 +1702,7 @@
         <v>16</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>1</v>
@@ -1766,36 +1763,36 @@
       <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>60</v>
+      <c r="D14" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="K14" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>29</v>
@@ -1858,7 +1855,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>1</v>
@@ -1878,18 +1875,18 @@
       <c r="I15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>29</v>
@@ -1951,39 +1948,39 @@
       <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>60</v>
+      <c r="D16" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="K16" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>29</v>
@@ -2049,7 +2046,7 @@
         <v>36</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2084,1227 +2081,539 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="W19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="X19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF19" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="19" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" s="2" t="s">
+      <c r="A20" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R20" s="2" t="s">
+      <c r="B20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="S20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="W20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="X20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF20" s="5" t="s">
-        <v>13</v>
+      <c r="C20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="U21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="W21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="X21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF21" s="5" t="s">
-        <v>13</v>
+      <c r="A21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U22" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V22" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="W22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="X22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF22" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="22" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M23" s="3"/>
-      <c r="N23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S23" s="3"/>
-      <c r="T23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="W23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="X23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF23" s="5" t="s">
-        <v>44</v>
+      <c r="A23" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S24" s="2"/>
-      <c r="T24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="U24" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="W24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="X24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF24" s="5" t="s">
-        <v>48</v>
+      <c r="A24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M25" s="3"/>
-      <c r="N25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S25" s="3"/>
-      <c r="T25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="U25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="W25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="X25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF25" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
+    <row r="25" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T26" s="3" t="s">
-        <v>46</v>
+      <c r="A26" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="U26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC26" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="11" t="s">
+    <row r="28" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R29" s="1" t="s">
+      <c r="K28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="S29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="U29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="V29" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="W29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z29" s="1" t="s">
+      <c r="AC28" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="S30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U30" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="V30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="W30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="X30" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z30" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC30" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE30" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="W32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="X32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y32" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z32" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="V33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="W33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="X33" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y33" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z33" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA33" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD33" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE33" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="T35" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="W35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X35" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y35" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC35" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="R37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="S37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="T37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="V37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA37" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB37" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC37" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update store text planning
</commit_message>
<xml_diff>
--- a/text/store.xlsx
+++ b/text/store.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="76">
   <si>
     <t xml:space="preserve">7E
 *
@@ -355,108 +355,6 @@
     <t xml:space="preserve">6A
 C
 0D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52</t>
   </si>
 </sst>
 </file>
@@ -496,7 +394,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -519,18 +417,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF8000"/>
         <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBE33D"/>
-        <bgColor rgb="FFFFCC00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4C7DC"/>
-        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -575,7 +461,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -608,32 +494,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -661,7 +527,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB4C7DC"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -689,7 +555,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FFBBE33D"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
@@ -713,15 +579,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF29"/>
+  <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T17" activeCellId="0" sqref="T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="1" style="1" width="6.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1014" min="1" style="1" width="6.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1015" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -1014,28 +880,28 @@
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="3" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="U4" s="4" t="s">
@@ -1226,7 +1092,7 @@
       <c r="T6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="U6" s="9" t="s">
+      <c r="U6" s="8" t="s">
         <v>1</v>
       </c>
       <c r="V6" s="6" t="s">
@@ -1270,7 +1136,7 @@
       <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1537,7 +1403,7 @@
       <c r="Q11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="R11" s="9" t="s">
         <v>59</v>
       </c>
       <c r="S11" s="2" t="s">
@@ -1682,38 +1548,38 @@
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="3" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="Q13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="U13" s="4" t="s">
@@ -1763,7 +1629,7 @@
       <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1857,54 +1723,54 @@
       <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3" t="s">
+      <c r="M15" s="3"/>
+      <c r="N15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P15" s="2" t="s">
+      <c r="P15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="Q15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="R15" s="2" t="s">
+      <c r="R15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S15" s="2"/>
-      <c r="T15" s="3" t="s">
+      <c r="S15" s="3"/>
+      <c r="T15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="U15" s="9" t="s">
+      <c r="U15" s="8" t="s">
         <v>1</v>
       </c>
       <c r="V15" s="6" t="s">
@@ -1948,10 +1814,10 @@
       <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2081,539 +1947,6 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="X21" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE21" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="X23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE24" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="U26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="V26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="X26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA26" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC26" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA28" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC28" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="36.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>